<commit_message>
Completed Insertion Sort and Selection Sort with chart data.
</commit_message>
<xml_diff>
--- a/Day 2/Manuj Grover - Complexity_Chart.xlsx
+++ b/Day 2/Manuj Grover - Complexity_Chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manuj\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Subjects\C with Linux\Assignments\Day 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923DC5AD-7253-4018-8522-F09F1C2EDAB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F2DEFD-2813-43D7-B1D5-1D53454C6F42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart" sheetId="1" r:id="rId1"/>
@@ -197,14 +197,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -230,6 +230,26 @@
   <c:style val="2"/>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IN"/>
+              <a:t>Bubble</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-IN" baseline="0"/>
+              <a:t> Sort</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-IN"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -700,6 +720,12 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+      </c:dTable>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
@@ -732,6 +758,2905 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IN"/>
+              <a:t>Insertion</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-IN" baseline="0"/>
+              <a:t> Sort</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$E$1:$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Insertion</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Random</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:softEdge rad="0"/>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Data!$A$3:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>28000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>36000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$E$3:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.33184000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75170999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.134689</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.214729</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.36464000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.41577700000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.548512</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.67150299999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8F05-40CB-B8A8-3967BB6E1E37}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$F$1:$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Insertion</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Asc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Data!$A$3:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>28000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>36000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$F$3:$F$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8F05-40CB-B8A8-3967BB6E1E37}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$G$1:$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Insertion</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Desc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Data!$A$3:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>28000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>36000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$G$3:$G$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.74170000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.4932799999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.26644800000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.426515</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.607064</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.8383849999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.1091167</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.1320527999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8F05-40CB-B8A8-3967BB6E1E37}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="677341631"/>
+        <c:axId val="677346623"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Data!$A$1:$A$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="2"/>
+                      <c:pt idx="0">
+                        <c:v>Input Size</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Data!$A$3:$A$11</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="9"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>8000</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>12000</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>16000</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>20000</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>24000</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>28000</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>32000</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>36000</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Data!$A$3:$A$11</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="9"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>8000</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>12000</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>16000</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>20000</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>24000</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>28000</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>32000</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>36000</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000003-8F05-40CB-B8A8-3967BB6E1E37}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="677341631"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IN"/>
+                  <a:t>Input</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-IN" baseline="0"/>
+                  <a:t> Size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="677346623"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="677346623"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IN"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-IN" baseline="0"/>
+                  <a:t>(seconds)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="677341631"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IN"/>
+              <a:t>Selection</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-IN" baseline="0"/>
+              <a:t> Sort</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-IN"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$N$1:$N$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Selection Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Random</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Data!$A$3:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>28000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>36000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$N$3:$N$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.67344000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1464</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2557119999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.406015</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.574864</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.785679</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1025775</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.1295151000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4BC7-4956-83FC-8D39943EC814}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$O$1:$O$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Selection Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Asc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Data!$A$3:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>28000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>36000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$O$3:$O$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.68320000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.14524000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.25667200000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.40406199999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.574883</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.7847040000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1022882000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.130296</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4BC7-4956-83FC-8D39943EC814}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$P$1:$P$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Selection Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Desc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Data!$A$3:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>28000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>36000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$P$3:$P$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.69298999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.15420800000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.27230399999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.42361100000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.60512100000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.8295939999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1076528000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.1375182000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4BC7-4956-83FC-8D39943EC814}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="957446783"/>
+        <c:axId val="957450527"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Data!$A$1:$A$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="2"/>
+                      <c:pt idx="0">
+                        <c:v>Input Size</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Data!$A$3:$A$11</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="9"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>8000</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>12000</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>16000</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>20000</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>24000</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>28000</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>32000</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>36000</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Data!$A$3:$A$11</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="9"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>8000</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>12000</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>16000</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>20000</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>24000</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>28000</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>32000</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>36000</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000003-4BC7-4956-83FC-8D39943EC814}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="957446783"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IN"/>
+                  <a:t>Input</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-IN" baseline="0"/>
+                  <a:t> Size</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-IN"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="957450527"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="957450527"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IN"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-IN" baseline="0"/>
+                  <a:t> (seconds)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-IN"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="957446783"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
@@ -741,7 +3666,7 @@
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="5695950" cy="3533775"/>
+    <xdr:ext cx="9304020" cy="4556760"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1" title="Chart">
@@ -765,6 +3690,82 @@
     </xdr:graphicFrame>
     <xdr:clientData fLocksWithSheet="0"/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>426720</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BAC84DB2-BD6B-44E3-98C8-466E59D50DEE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>434340</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3A56BB0-8C06-4A92-BA3A-B78379EFFF37}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -968,8 +3969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K65" sqref="K65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1990,8 +4991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2000,9 +5001,9 @@
     <col min="2" max="2" width="13.44140625" customWidth="1"/>
     <col min="3" max="3" width="12.5546875" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" customWidth="1"/>
     <col min="6" max="6" width="8.109375" customWidth="1"/>
-    <col min="7" max="7" width="7.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13.21875" customWidth="1"/>
     <col min="8" max="8" width="8.109375" customWidth="1"/>
     <col min="9" max="9" width="8.6640625" customWidth="1"/>
     <col min="10" max="11" width="7.88671875" customWidth="1"/>
@@ -2014,37 +5015,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="12" t="s">
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="12" t="s">
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="12" t="s">
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="12" t="s">
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
+      <c r="A2" s="13"/>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
@@ -2104,18 +5105,30 @@
       <c r="D3" s="3">
         <v>0</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0</v>
+      </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
+      <c r="N3" s="2">
+        <v>0</v>
+      </c>
+      <c r="O3" s="2">
+        <v>0</v>
+      </c>
+      <c r="P3" s="2">
+        <v>0</v>
+      </c>
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
@@ -2140,18 +5153,30 @@
       <c r="D4" s="6">
         <v>0.15612000000000001</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
+      <c r="E4" s="5">
+        <v>0.33184000000000002</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0.74170000000000003</v>
+      </c>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
+      <c r="N4" s="5">
+        <v>0.67344000000000004</v>
+      </c>
+      <c r="O4" s="5">
+        <v>0.68320000000000003</v>
+      </c>
+      <c r="P4" s="5">
+        <v>0.69298999999999999</v>
+      </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
@@ -2166,18 +5191,30 @@
       <c r="D5" s="8">
         <v>0.33659</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
+      <c r="E5" s="7">
+        <v>0.75170999999999999</v>
+      </c>
+      <c r="F5" s="7">
+        <v>0</v>
+      </c>
+      <c r="G5" s="7">
+        <v>1.4932799999999999</v>
+      </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
+      <c r="N5" s="7">
+        <v>0.1464</v>
+      </c>
+      <c r="O5" s="7">
+        <v>0.14524000000000001</v>
+      </c>
+      <c r="P5" s="7">
+        <v>0.15420800000000001</v>
+      </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
@@ -2192,18 +5229,30 @@
       <c r="D6" s="8">
         <v>0.592275</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
+      <c r="E6" s="7">
+        <v>0.134689</v>
+      </c>
+      <c r="F6" s="7">
+        <v>0</v>
+      </c>
+      <c r="G6" s="7">
+        <v>0.26644800000000002</v>
+      </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
+      <c r="N6" s="7">
+        <v>1.2557119999999999</v>
+      </c>
+      <c r="O6" s="7">
+        <v>0.25667200000000001</v>
+      </c>
+      <c r="P6" s="7">
+        <v>0.27230399999999999</v>
+      </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
@@ -2218,18 +5267,30 @@
       <c r="D7" s="8">
         <v>1.9218189999999999</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
+      <c r="E7" s="7">
+        <v>0.214729</v>
+      </c>
+      <c r="F7" s="7">
+        <v>0</v>
+      </c>
+      <c r="G7" s="7">
+        <v>1.426515</v>
+      </c>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
+      <c r="N7" s="7">
+        <v>1.406015</v>
+      </c>
+      <c r="O7" s="7">
+        <v>0.40406199999999998</v>
+      </c>
+      <c r="P7" s="7">
+        <v>0.42361100000000002</v>
+      </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
@@ -2244,18 +5305,30 @@
       <c r="D8" s="8">
         <v>1.1346924</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
+      <c r="E8" s="7">
+        <v>0.36464000000000002</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0</v>
+      </c>
+      <c r="G8" s="7">
+        <v>1.607064</v>
+      </c>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
       <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
+      <c r="N8" s="7">
+        <v>1.574864</v>
+      </c>
+      <c r="O8" s="7">
+        <v>1.574883</v>
+      </c>
+      <c r="P8" s="7">
+        <v>0.60512100000000002</v>
+      </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
@@ -2270,18 +5343,30 @@
       <c r="D9" s="8">
         <v>2.1869079</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
+      <c r="E9" s="7">
+        <v>0.41577700000000001</v>
+      </c>
+      <c r="F9" s="7">
+        <v>0</v>
+      </c>
+      <c r="G9" s="7">
+        <v>1.8383849999999999</v>
+      </c>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
+      <c r="N9" s="7">
+        <v>1.785679</v>
+      </c>
+      <c r="O9" s="7">
+        <v>1.7847040000000001</v>
+      </c>
+      <c r="P9" s="7">
+        <v>1.8295939999999999</v>
+      </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
@@ -2296,18 +5381,30 @@
       <c r="D10" s="8">
         <v>3.2617403999999999</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
+      <c r="E10" s="7">
+        <v>0.548512</v>
+      </c>
+      <c r="F10" s="7">
+        <v>0</v>
+      </c>
+      <c r="G10" s="7">
+        <v>2.1091167</v>
+      </c>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
+      <c r="N10" s="7">
+        <v>1.1025775</v>
+      </c>
+      <c r="O10" s="7">
+        <v>1.1022882000000001</v>
+      </c>
+      <c r="P10" s="7">
+        <v>1.1076528000000001</v>
+      </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
@@ -2322,18 +5419,30 @@
       <c r="D11" s="8">
         <v>3.2977131000000002</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
+      <c r="E11" s="7">
+        <v>0.67150299999999996</v>
+      </c>
+      <c r="F11" s="7">
+        <v>0</v>
+      </c>
+      <c r="G11" s="7">
+        <v>2.1320527999999999</v>
+      </c>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
+      <c r="N11" s="7">
+        <v>1.1295151000000001</v>
+      </c>
+      <c r="O11" s="7">
+        <v>1.130296</v>
+      </c>
+      <c r="P11" s="7">
+        <v>2.1375182000000001</v>
+      </c>
     </row>
     <row r="12" spans="1:26" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M12" s="9"/>

</xml_diff>